<commit_message>
Initalized all the framework xaml files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyComputer\Documents\UiPath\ReFrameWork-master\New folder\UiPath_REFrameWork_UiDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A06C051-356D-4D79-BA90-804D37AB6ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4771D087-403C-43AF-ADF9-49A24F561493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,9 +165,6 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>QueueName</t>
-  </si>
-  <si>
     <t>readData</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>UiDemoPath</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -587,10 +587,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -598,13 +598,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1614,6 +1614,7 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2839,7 +2840,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="65.44140625" customWidth="1"/>
+    <col min="2" max="2" width="71.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2878,10 +2881,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Stable version of uidemo
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyComputer\Documents\UiPath\ReFrameWork-master\New folder\UiPath_REFrameWork_UiDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4771D087-403C-43AF-ADF9-49A24F561493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883141E0-18B2-4F52-ACF9-2F87BE0E185A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -168,12 +168,6 @@
     <t>readData</t>
   </si>
   <si>
-    <t>UIDemoCredential</t>
-  </si>
-  <si>
-    <t>UIDemoCredential_Framework</t>
-  </si>
-  <si>
     <t>Credential used to log in to UIDemo</t>
   </si>
   <si>
@@ -181,6 +175,9 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>UiDemoCredential</t>
   </si>
 </sst>
 </file>
@@ -539,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -587,7 +584,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -598,13 +595,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2832,10 +2829,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2881,10 +2878,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3884,7 +3881,6 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>